<commit_message>
add navigation header and import attempt/list page
</commit_message>
<xml_diff>
--- a/2013_calendar.xlsx
+++ b/2013_calendar.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="10230" yWindow="105" windowWidth="10275" windowHeight="6555"/>
@@ -16,12 +16,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Notes!$B$14:$F$127</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schedule!$B$3:$G$118</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0" concurrentManualCount="1"/>
+  <calcPr calcId="144525" concurrentCalc="0" concurrentManualCount="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="78">
   <si>
     <t>Dates not available</t>
   </si>
@@ -264,13 +264,10 @@
     <t>Canceled</t>
   </si>
   <si>
-    <t>Cancel BC on the 27th?</t>
-  </si>
-  <si>
-    <t>Cancel BC on the 23rd?</t>
-  </si>
-  <si>
     <t>DateTime</t>
+  </si>
+  <si>
+    <t>Title</t>
   </si>
 </sst>
 </file>
@@ -279,8 +276,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="168" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -444,11 +441,11 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,7 +753,7 @@
   <dimension ref="B1:I130"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,20 +766,21 @@
     <col min="6" max="6" width="35" customWidth="1"/>
     <col min="7" max="7" width="54.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="50.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+    <row r="1" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-    </row>
-    <row r="2" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+    </row>
+    <row r="2" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:9" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
@@ -790,7 +788,7 @@
         <v>6</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>7</v>
@@ -804,15 +802,18 @@
       <c r="H3" s="8" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>41455</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="40">
         <v>0.4375</v>
       </c>
-      <c r="D4" s="42">
+      <c r="D4" s="41">
         <f>B4+C4</f>
         <v>41455.4375</v>
       </c>
@@ -825,15 +826,19 @@
       <c r="H4" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="5" t="str">
+        <f>CONCATENATE(F4," - ",E4)</f>
+        <v>Service - Jouko Haapsaari</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>41455</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="40">
         <v>0.47916666666666702</v>
       </c>
-      <c r="D5" s="42">
+      <c r="D5" s="41">
         <f t="shared" ref="D5:D68" si="0">B5+C5</f>
         <v>41455.479166666664</v>
       </c>
@@ -846,15 +851,19 @@
       <c r="H5" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="5" t="str">
+        <f t="shared" ref="I5:I68" si="1">CONCATENATE(F5," - ",E5)</f>
+        <v>Service - Mark Lee</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>41458</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="40">
         <v>0.52083333333333304</v>
       </c>
-      <c r="D6" s="42">
+      <c r="D6" s="41">
         <f t="shared" si="0"/>
         <v>41458.520833333336</v>
       </c>
@@ -867,15 +876,19 @@
       <c r="H6" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Song Services - Rocky Sorvala</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>41462</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="40">
         <v>0.5625</v>
       </c>
-      <c r="D7" s="42">
+      <c r="D7" s="41">
         <f t="shared" si="0"/>
         <v>41462.5625</v>
       </c>
@@ -885,15 +898,19 @@
       <c r="H7" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Nathan Muhonen</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="17">
         <v>41462</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C8" s="40">
         <v>0.60416666666666696</v>
       </c>
-      <c r="D8" s="42">
+      <c r="D8" s="41">
         <f t="shared" si="0"/>
         <v>41462.604166666664</v>
       </c>
@@ -906,15 +923,19 @@
       <c r="G8" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>LLCM - Mark Lee</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3">
         <v>41462</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="40">
         <v>0.64583333333333304</v>
       </c>
-      <c r="D9" s="42">
+      <c r="D9" s="41">
         <f t="shared" si="0"/>
         <v>41462.645833333336</v>
       </c>
@@ -924,15 +945,19 @@
       <c r="H9" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Joe Lehtola</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9">
         <v>41465</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C10" s="40">
         <v>0.6875</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="41">
         <f t="shared" si="0"/>
         <v>41465.6875</v>
       </c>
@@ -944,15 +969,19 @@
       <c r="H10" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="33">
         <v>41467</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="40">
         <v>0.72916666666666696</v>
       </c>
-      <c r="D11" s="42">
+      <c r="D11" s="41">
         <f t="shared" si="0"/>
         <v>41467.729166666664</v>
       </c>
@@ -966,15 +995,19 @@
         <v>73</v>
       </c>
       <c r="H11" s="32"/>
-    </row>
-    <row r="12" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Finnish Service - Olli Lohi</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>41469</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="40">
         <v>0.77083333333333304</v>
       </c>
-      <c r="D12" s="42">
+      <c r="D12" s="41">
         <f t="shared" si="0"/>
         <v>41469.770833333336</v>
       </c>
@@ -987,15 +1020,19 @@
       <c r="H12" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Service (Rotation Sunday) - Jeremy Honga</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>41469</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="40">
         <v>0.8125</v>
       </c>
-      <c r="D13" s="42">
+      <c r="D13" s="41">
         <f t="shared" si="0"/>
         <v>41469.8125</v>
       </c>
@@ -1005,15 +1042,19 @@
       <c r="H13" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Rick Nevala</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9">
         <v>41472</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="40">
         <v>0.85416666666666696</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="41">
         <f t="shared" si="0"/>
         <v>41472.854166666664</v>
       </c>
@@ -1025,15 +1066,19 @@
       <c r="H14" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>41476</v>
       </c>
-      <c r="C15" s="41">
+      <c r="C15" s="40">
         <v>0.89583333333333304</v>
       </c>
-      <c r="D15" s="42">
+      <c r="D15" s="41">
         <f t="shared" si="0"/>
         <v>41476.895833333336</v>
       </c>
@@ -1043,15 +1088,19 @@
       <c r="H15" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Rocky Sorvala</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3">
         <v>41476</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="40">
         <v>0.9375</v>
       </c>
-      <c r="D16" s="42">
+      <c r="D16" s="41">
         <f t="shared" si="0"/>
         <v>41476.9375</v>
       </c>
@@ -1067,15 +1116,19 @@
       <c r="H16" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Evening Service - Mikko Tahkola</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="9">
         <v>41479</v>
       </c>
-      <c r="C17" s="41">
+      <c r="C17" s="40">
         <v>0.97916666666666696</v>
       </c>
-      <c r="D17" s="42">
+      <c r="D17" s="41">
         <f t="shared" si="0"/>
         <v>41479.979166666664</v>
       </c>
@@ -1087,15 +1140,19 @@
       <c r="H17" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I17" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="36">
         <v>41480</v>
       </c>
-      <c r="C18" s="41">
+      <c r="C18" s="40">
         <v>1.0208333333333299</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="41">
         <f t="shared" si="0"/>
         <v>41481.020833333336</v>
       </c>
@@ -1111,15 +1168,19 @@
       <c r="H18" s="37" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Finnish Service - Olli Lohi</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>41483</v>
       </c>
-      <c r="C19" s="41">
+      <c r="C19" s="40">
         <v>1.0625</v>
       </c>
-      <c r="D19" s="42">
+      <c r="D19" s="41">
         <f t="shared" si="0"/>
         <v>41484.0625</v>
       </c>
@@ -1129,15 +1190,19 @@
       <c r="H19" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Joe Lehtola</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>41483</v>
       </c>
-      <c r="C20" s="41">
+      <c r="C20" s="40">
         <v>1.1041666666666701</v>
       </c>
-      <c r="D20" s="42">
+      <c r="D20" s="41">
         <f t="shared" si="0"/>
         <v>41484.104166666664</v>
       </c>
@@ -1147,15 +1212,19 @@
       <c r="H20" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Jouko Haapsaari</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="17">
         <v>41483</v>
       </c>
-      <c r="C21" s="41">
+      <c r="C21" s="40">
         <v>1.1458333333333299</v>
       </c>
-      <c r="D21" s="42">
+      <c r="D21" s="41">
         <f t="shared" si="0"/>
         <v>41484.145833333336</v>
       </c>
@@ -1168,15 +1237,19 @@
       <c r="G21" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>LLCM - Ray Waaraniemi</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="22">
         <v>41483</v>
       </c>
-      <c r="C22" s="41">
+      <c r="C22" s="40">
         <v>1.1875</v>
       </c>
-      <c r="D22" s="42">
+      <c r="D22" s="41">
         <f t="shared" si="0"/>
         <v>41484.1875</v>
       </c>
@@ -1192,15 +1265,19 @@
       <c r="H22" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Annandale Nursing Home  - Craig Kumpula</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="3">
         <v>41484</v>
       </c>
-      <c r="C23" s="41">
+      <c r="C23" s="40">
         <v>1.2291666666666701</v>
       </c>
-      <c r="D23" s="42">
+      <c r="D23" s="41">
         <f t="shared" si="0"/>
         <v>41485.229166666664</v>
       </c>
@@ -1216,15 +1293,19 @@
       <c r="H23" s="31" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="24" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Finnish Service - Tapani Kinnunen</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="9">
         <v>41486</v>
       </c>
-      <c r="C24" s="41">
+      <c r="C24" s="40">
         <v>1.2708333333333299</v>
       </c>
-      <c r="D24" s="42">
+      <c r="D24" s="41">
         <f t="shared" si="0"/>
         <v>41487.270833333336</v>
       </c>
@@ -1236,15 +1317,19 @@
       <c r="H24" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
         <v>41490</v>
       </c>
-      <c r="C25" s="41">
+      <c r="C25" s="40">
         <v>1.3125</v>
       </c>
-      <c r="D25" s="42">
+      <c r="D25" s="41">
         <f t="shared" si="0"/>
         <v>41491.3125</v>
       </c>
@@ -1254,15 +1339,19 @@
       <c r="H25" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="26" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Jouko Haapsaari</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="3">
         <v>41490</v>
       </c>
-      <c r="C26" s="41">
+      <c r="C26" s="40">
         <v>1.3541666666666701</v>
       </c>
-      <c r="D26" s="42">
+      <c r="D26" s="41">
         <f t="shared" si="0"/>
         <v>41491.354166666664</v>
       </c>
@@ -1272,15 +1361,19 @@
       <c r="H26" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Ray Waaraniemi</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="3">
         <v>41493</v>
       </c>
-      <c r="C27" s="41">
+      <c r="C27" s="40">
         <v>1.3958333333333299</v>
       </c>
-      <c r="D27" s="42">
+      <c r="D27" s="41">
         <f t="shared" si="0"/>
         <v>41494.395833333336</v>
       </c>
@@ -1293,15 +1386,19 @@
       <c r="H27" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="28" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Song Services - Randy Herrala</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="3">
         <v>41497</v>
       </c>
-      <c r="C28" s="41">
+      <c r="C28" s="40">
         <v>1.4375</v>
       </c>
-      <c r="D28" s="42">
+      <c r="D28" s="41">
         <f t="shared" si="0"/>
         <v>41498.4375</v>
       </c>
@@ -1311,15 +1408,19 @@
       <c r="H28" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Rod Nikula</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17">
         <v>41497</v>
       </c>
-      <c r="C29" s="41">
+      <c r="C29" s="40">
         <v>1.4791666666666701</v>
       </c>
-      <c r="D29" s="42">
+      <c r="D29" s="41">
         <f t="shared" si="0"/>
         <v>41498.479166666664</v>
       </c>
@@ -1332,15 +1433,19 @@
       <c r="G29" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="30" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>LLCM - Joe Lehtola</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="3">
         <v>41497</v>
       </c>
-      <c r="C30" s="41">
+      <c r="C30" s="40">
         <v>1.5208333333333299</v>
       </c>
-      <c r="D30" s="42">
+      <c r="D30" s="41">
         <f t="shared" si="0"/>
         <v>41498.520833333336</v>
       </c>
@@ -1350,15 +1455,19 @@
       <c r="H30" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="31" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Nathan Muhonen</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="9">
         <v>41500</v>
       </c>
-      <c r="C31" s="41">
+      <c r="C31" s="40">
         <v>1.5625</v>
       </c>
-      <c r="D31" s="42">
+      <c r="D31" s="41">
         <f t="shared" si="0"/>
         <v>41501.5625</v>
       </c>
@@ -1370,15 +1479,19 @@
       <c r="H31" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I31" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="14">
         <v>41502</v>
       </c>
-      <c r="C32" s="41">
+      <c r="C32" s="40">
         <v>1.6041666666666701</v>
       </c>
-      <c r="D32" s="42">
+      <c r="D32" s="41">
         <f t="shared" si="0"/>
         <v>41503.604166666664</v>
       </c>
@@ -1391,15 +1504,19 @@
       <c r="G32" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>RLLC Youth Days - M. Wittenberg; K. Moll</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="14">
         <v>41503</v>
       </c>
-      <c r="C33" s="41">
+      <c r="C33" s="40">
         <v>1.6458333333333299</v>
       </c>
-      <c r="D33" s="42">
+      <c r="D33" s="41">
         <f t="shared" si="0"/>
         <v>41504.645833333336</v>
       </c>
@@ -1412,15 +1529,19 @@
       <c r="G33" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>RLLC Youth Days - M. Wittenberg; K. Moll</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="14">
         <v>41503</v>
       </c>
-      <c r="C34" s="41">
+      <c r="C34" s="40">
         <v>1.6875</v>
       </c>
-      <c r="D34" s="42">
+      <c r="D34" s="41">
         <f t="shared" si="0"/>
         <v>41504.6875</v>
       </c>
@@ -1433,15 +1554,19 @@
       <c r="G34" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I34" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>RLLC Youth Days - M. Wittenberg; K. Moll</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="14">
         <v>41504</v>
       </c>
-      <c r="C35" s="41">
+      <c r="C35" s="40">
         <v>1.7291666666666701</v>
       </c>
-      <c r="D35" s="42">
+      <c r="D35" s="41">
         <f t="shared" si="0"/>
         <v>41505.729166666664</v>
       </c>
@@ -1457,15 +1582,19 @@
       <c r="H35" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>RLLC Youth Days - Russ Roiko</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="14">
         <v>41504</v>
       </c>
-      <c r="C36" s="41">
+      <c r="C36" s="40">
         <v>1.7708333333333299</v>
       </c>
-      <c r="D36" s="42">
+      <c r="D36" s="41">
         <f t="shared" si="0"/>
         <v>41505.770833333336</v>
       </c>
@@ -1478,15 +1607,19 @@
       <c r="G36" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="37" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>RLLC Youth Days - M. Wittenberg; K. Moll</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="14">
         <v>41504</v>
       </c>
-      <c r="C37" s="41">
+      <c r="C37" s="40">
         <v>1.8125</v>
       </c>
-      <c r="D37" s="42">
+      <c r="D37" s="41">
         <f t="shared" si="0"/>
         <v>41505.8125</v>
       </c>
@@ -1499,15 +1632,19 @@
       <c r="G37" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="38" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>RLLC Youth Days - M. Wittenberg; K. Moll</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="14">
         <v>41504</v>
       </c>
-      <c r="C38" s="41">
+      <c r="C38" s="40">
         <v>1.8541666666666701</v>
       </c>
-      <c r="D38" s="42">
+      <c r="D38" s="41">
         <f t="shared" si="0"/>
         <v>41505.854166666664</v>
       </c>
@@ -1520,15 +1657,19 @@
       <c r="G38" s="16" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="39" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I38" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>RLLC Youth Days - Jouko Haapsaari</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="9">
         <v>41507</v>
       </c>
-      <c r="C39" s="41">
+      <c r="C39" s="40">
         <v>1.8958333333333299</v>
       </c>
-      <c r="D39" s="42">
+      <c r="D39" s="41">
         <f t="shared" si="0"/>
         <v>41508.895833333336</v>
       </c>
@@ -1540,15 +1681,19 @@
       <c r="H39" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="40" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I39" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="3">
         <v>41511</v>
       </c>
-      <c r="C40" s="41">
+      <c r="C40" s="40">
         <v>1.9375</v>
       </c>
-      <c r="D40" s="42">
+      <c r="D40" s="41">
         <f t="shared" si="0"/>
         <v>41512.9375</v>
       </c>
@@ -1558,15 +1703,19 @@
       <c r="H40" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="41" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I40" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Rick Nevala</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
         <v>41511</v>
       </c>
-      <c r="C41" s="41">
+      <c r="C41" s="40">
         <v>1.9791666666666701</v>
       </c>
-      <c r="D41" s="42">
+      <c r="D41" s="41">
         <f t="shared" si="0"/>
         <v>41512.979166666664</v>
       </c>
@@ -1576,15 +1725,19 @@
       <c r="H41" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="42" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I41" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Ray Waaraniemi</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="9">
         <v>41514</v>
       </c>
-      <c r="C42" s="41">
+      <c r="C42" s="40">
         <v>2.0208333333333299</v>
       </c>
-      <c r="D42" s="42">
+      <c r="D42" s="41">
         <f t="shared" si="0"/>
         <v>41516.020833333336</v>
       </c>
@@ -1596,15 +1749,19 @@
       <c r="H42" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="43" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I42" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
         <v>41518</v>
       </c>
-      <c r="C43" s="41">
+      <c r="C43" s="40">
         <v>2.0625</v>
       </c>
-      <c r="D43" s="42">
+      <c r="D43" s="41">
         <f t="shared" si="0"/>
         <v>41520.0625</v>
       </c>
@@ -1614,15 +1771,19 @@
       <c r="H43" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="44" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I43" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Jouko Haapsaari</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="3">
         <v>41518</v>
       </c>
-      <c r="C44" s="41">
+      <c r="C44" s="40">
         <v>2.1041666666666701</v>
       </c>
-      <c r="D44" s="42">
+      <c r="D44" s="41">
         <f t="shared" si="0"/>
         <v>41520.104166666664</v>
       </c>
@@ -1632,15 +1793,19 @@
       <c r="H44" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="45" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I44" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Rocky Sorvala</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
         <v>41521</v>
       </c>
-      <c r="C45" s="41">
+      <c r="C45" s="40">
         <v>2.1458333333333299</v>
       </c>
-      <c r="D45" s="42">
+      <c r="D45" s="41">
         <f t="shared" si="0"/>
         <v>41523.145833333336</v>
       </c>
@@ -1653,15 +1818,19 @@
       <c r="H45" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="46" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I45" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Song Services - Mark Lee</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="3">
         <v>41525</v>
       </c>
-      <c r="C46" s="41">
+      <c r="C46" s="40">
         <v>2.1875</v>
       </c>
-      <c r="D46" s="42">
+      <c r="D46" s="41">
         <f t="shared" si="0"/>
         <v>41527.1875</v>
       </c>
@@ -1671,15 +1840,19 @@
       <c r="H46" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="47" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Nathan Muhonen</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="17">
         <v>41525</v>
       </c>
-      <c r="C47" s="41">
+      <c r="C47" s="40">
         <v>2.2291666666666701</v>
       </c>
-      <c r="D47" s="42">
+      <c r="D47" s="41">
         <f t="shared" si="0"/>
         <v>41527.229166666664</v>
       </c>
@@ -1692,15 +1865,19 @@
       <c r="G47" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="48" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I47" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>LLCM - Jouko Haapsaari</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="3">
         <v>41525</v>
       </c>
-      <c r="C48" s="41">
+      <c r="C48" s="40">
         <v>2.2708333333333299</v>
       </c>
-      <c r="D48" s="42">
+      <c r="D48" s="41">
         <f t="shared" si="0"/>
         <v>41527.270833333336</v>
       </c>
@@ -1710,15 +1887,19 @@
       <c r="H48" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Rod Nikula</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="9">
         <v>41528</v>
       </c>
-      <c r="C49" s="41">
+      <c r="C49" s="40">
         <v>2.3125</v>
       </c>
-      <c r="D49" s="42">
+      <c r="D49" s="41">
         <f t="shared" si="0"/>
         <v>41530.3125</v>
       </c>
@@ -1730,15 +1911,19 @@
       <c r="H49" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="50" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="3">
         <v>41532</v>
       </c>
-      <c r="C50" s="41">
+      <c r="C50" s="40">
         <v>2.3541666666666701</v>
       </c>
-      <c r="D50" s="42">
+      <c r="D50" s="41">
         <f t="shared" si="0"/>
         <v>41534.354166666664</v>
       </c>
@@ -1751,15 +1936,19 @@
       <c r="H50" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="51" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Service (Rotation Sunday) - Travis Ruonavaara</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="3">
         <v>41532</v>
       </c>
-      <c r="C51" s="41">
+      <c r="C51" s="40">
         <v>2.3958333333333299</v>
       </c>
-      <c r="D51" s="42">
+      <c r="D51" s="41">
         <f t="shared" si="0"/>
         <v>41534.395833333336</v>
       </c>
@@ -1769,15 +1958,19 @@
       <c r="H51" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="52" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I51" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Jouko Haapsaari</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="9">
         <v>41535</v>
       </c>
-      <c r="C52" s="41">
+      <c r="C52" s="40">
         <v>2.4375</v>
       </c>
-      <c r="D52" s="42">
+      <c r="D52" s="41">
         <f t="shared" si="0"/>
         <v>41537.4375</v>
       </c>
@@ -1789,15 +1982,19 @@
       <c r="H52" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="53" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I52" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="3">
         <v>41539</v>
       </c>
-      <c r="C53" s="41">
+      <c r="C53" s="40">
         <v>2.4791666666666701</v>
       </c>
-      <c r="D53" s="42">
+      <c r="D53" s="41">
         <f t="shared" si="0"/>
         <v>41541.479166666664</v>
       </c>
@@ -1807,15 +2004,19 @@
       <c r="H53" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I53" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Randy Herrala</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="3">
         <v>41539</v>
       </c>
-      <c r="C54" s="41">
+      <c r="C54" s="40">
         <v>2.5208333333333299</v>
       </c>
-      <c r="D54" s="42">
+      <c r="D54" s="41">
         <f t="shared" si="0"/>
         <v>41541.520833333336</v>
       </c>
@@ -1825,15 +2026,19 @@
       <c r="H54" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="55" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I54" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Rick Nevala</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="9">
         <v>41542</v>
       </c>
-      <c r="C55" s="41">
+      <c r="C55" s="40">
         <v>2.5625</v>
       </c>
-      <c r="D55" s="42">
+      <c r="D55" s="41">
         <f t="shared" si="0"/>
         <v>41544.5625</v>
       </c>
@@ -1845,15 +2050,19 @@
       <c r="H55" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="56" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I55" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="3">
         <v>41546</v>
       </c>
-      <c r="C56" s="41">
+      <c r="C56" s="40">
         <v>2.6041666666666701</v>
       </c>
-      <c r="D56" s="42">
+      <c r="D56" s="41">
         <f t="shared" si="0"/>
         <v>41548.604166666664</v>
       </c>
@@ -1863,15 +2072,19 @@
       <c r="H56" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="57" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I56" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Craig Kumpula</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="22">
         <v>41546</v>
       </c>
-      <c r="C57" s="41">
+      <c r="C57" s="40">
         <v>2.6458333333333299</v>
       </c>
-      <c r="D57" s="42">
+      <c r="D57" s="41">
         <f t="shared" si="0"/>
         <v>41548.645833333336</v>
       </c>
@@ -1887,15 +2100,19 @@
       <c r="H57" s="24" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="58" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I57" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Annandale Nursing Home  - Rod Nikula</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="3">
         <v>41546</v>
       </c>
-      <c r="C58" s="41">
+      <c r="C58" s="40">
         <v>2.6875</v>
       </c>
-      <c r="D58" s="42">
+      <c r="D58" s="41">
         <f t="shared" si="0"/>
         <v>41548.6875</v>
       </c>
@@ -1905,15 +2122,19 @@
       <c r="H58" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="59" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I58" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Mark Lee</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="17">
         <v>41546</v>
       </c>
-      <c r="C59" s="41">
+      <c r="C59" s="40">
         <v>2.7291666666666701</v>
       </c>
-      <c r="D59" s="42">
+      <c r="D59" s="41">
         <f t="shared" si="0"/>
         <v>41548.729166666664</v>
       </c>
@@ -1926,15 +2147,19 @@
       <c r="G59" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="60" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I59" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>LLCM - Nathan Muhonen</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="9">
         <v>41549</v>
       </c>
-      <c r="C60" s="41">
+      <c r="C60" s="40">
         <v>2.7708333333333299</v>
       </c>
-      <c r="D60" s="42">
+      <c r="D60" s="41">
         <f t="shared" si="0"/>
         <v>41551.770833333336</v>
       </c>
@@ -1946,15 +2171,19 @@
       <c r="H60" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="61" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I60" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Home Services - </v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="3">
         <v>41553</v>
       </c>
-      <c r="C61" s="41">
+      <c r="C61" s="40">
         <v>2.8125</v>
       </c>
-      <c r="D61" s="42">
+      <c r="D61" s="41">
         <f t="shared" si="0"/>
         <v>41555.8125</v>
       </c>
@@ -1964,15 +2193,19 @@
       <c r="H61" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="62" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I61" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Rocky Sorvala</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="3">
         <v>41553</v>
       </c>
-      <c r="C62" s="41">
+      <c r="C62" s="40">
         <v>2.8541666666666701</v>
       </c>
-      <c r="D62" s="42">
+      <c r="D62" s="41">
         <f t="shared" si="0"/>
         <v>41555.854166666664</v>
       </c>
@@ -1982,15 +2215,19 @@
       <c r="H62" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="63" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I62" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Joe Lehtola</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="9">
         <v>41556</v>
       </c>
-      <c r="C63" s="41">
+      <c r="C63" s="40">
         <v>2.8958333333333299</v>
       </c>
-      <c r="D63" s="42">
+      <c r="D63" s="41">
         <f t="shared" si="0"/>
         <v>41558.895833333336</v>
       </c>
@@ -2002,15 +2239,19 @@
       <c r="H63" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="64" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I63" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="3">
         <v>41560</v>
       </c>
-      <c r="C64" s="41">
+      <c r="C64" s="40">
         <v>2.9375</v>
       </c>
-      <c r="D64" s="42">
+      <c r="D64" s="41">
         <f t="shared" si="0"/>
         <v>41562.9375</v>
       </c>
@@ -2022,16 +2263,20 @@
       </c>
       <c r="H64" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I64" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>Service (Rotation Sunday) - Jim Jurmu</v>
       </c>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="17">
         <v>41560</v>
       </c>
-      <c r="C65" s="41">
+      <c r="C65" s="40">
         <v>2.9791666666666701</v>
       </c>
-      <c r="D65" s="42">
+      <c r="D65" s="41">
         <f t="shared" si="0"/>
         <v>41562.979166666664</v>
       </c>
@@ -2043,16 +2288,20 @@
       </c>
       <c r="G65" s="19" t="s">
         <v>52</v>
+      </c>
+      <c r="I65" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>LLCM - Ray Waaraniemi</v>
       </c>
     </row>
     <row r="66" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="3">
         <v>41560</v>
       </c>
-      <c r="C66" s="41">
+      <c r="C66" s="40">
         <v>3.0208333333333299</v>
       </c>
-      <c r="D66" s="42">
+      <c r="D66" s="41">
         <f t="shared" si="0"/>
         <v>41563.020833333336</v>
       </c>
@@ -2061,16 +2310,20 @@
       </c>
       <c r="H66" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I66" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Nathan Muhonen</v>
       </c>
     </row>
     <row r="67" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="9">
         <v>41563</v>
       </c>
-      <c r="C67" s="41">
+      <c r="C67" s="40">
         <v>3.0625</v>
       </c>
-      <c r="D67" s="42">
+      <c r="D67" s="41">
         <f t="shared" si="0"/>
         <v>41566.0625</v>
       </c>
@@ -2081,15 +2334,19 @@
       <c r="H67" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="I67" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
     </row>
     <row r="68" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="3">
         <v>41567</v>
       </c>
-      <c r="C68" s="41">
+      <c r="C68" s="40">
         <v>3.1041666666666701</v>
       </c>
-      <c r="D68" s="42">
+      <c r="D68" s="41">
         <f t="shared" si="0"/>
         <v>41570.104166666664</v>
       </c>
@@ -2101,17 +2358,21 @@
       </c>
       <c r="H68" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I68" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> - Archived Sermon</v>
       </c>
     </row>
     <row r="69" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="3">
         <v>41567</v>
       </c>
-      <c r="C69" s="41">
+      <c r="C69" s="40">
         <v>3.1458333333333299</v>
       </c>
-      <c r="D69" s="42">
-        <f t="shared" ref="D69:D118" si="1">B69+C69</f>
+      <c r="D69" s="41">
+        <f t="shared" ref="D69:D118" si="2">B69+C69</f>
         <v>41570.145833333336</v>
       </c>
       <c r="E69" s="12" t="s">
@@ -2122,17 +2383,21 @@
       </c>
       <c r="H69" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I69" s="5" t="str">
+        <f t="shared" ref="I69:I118" si="3">CONCATENATE(F69," - ",E69)</f>
+        <v xml:space="preserve"> - Archived Sermon</v>
       </c>
     </row>
     <row r="70" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="9">
         <v>41570</v>
       </c>
-      <c r="C70" s="41">
+      <c r="C70" s="40">
         <v>3.1875</v>
       </c>
-      <c r="D70" s="42">
-        <f t="shared" si="1"/>
+      <c r="D70" s="41">
+        <f t="shared" si="2"/>
         <v>41573.1875</v>
       </c>
       <c r="E70" s="11"/>
@@ -2142,16 +2407,20 @@
       <c r="H70" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="I70" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
     </row>
     <row r="71" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="38">
         <v>41571</v>
       </c>
-      <c r="C71" s="41">
+      <c r="C71" s="40">
         <v>3.2291666666666701</v>
       </c>
-      <c r="D71" s="42">
-        <f t="shared" si="1"/>
+      <c r="D71" s="41">
+        <f t="shared" si="2"/>
         <v>41574.229166666664</v>
       </c>
       <c r="E71" s="5" t="s">
@@ -2163,19 +2432,20 @@
       <c r="H71" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="I71" s="30" t="s">
-        <v>77</v>
+      <c r="I71" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Finnish Service - Esa Koukkari</v>
       </c>
     </row>
     <row r="72" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="3">
         <v>41574</v>
       </c>
-      <c r="C72" s="41">
+      <c r="C72" s="40">
         <v>3.2708333333333299</v>
       </c>
-      <c r="D72" s="42">
-        <f t="shared" si="1"/>
+      <c r="D72" s="41">
+        <f t="shared" si="2"/>
         <v>41577.270833333336</v>
       </c>
       <c r="E72" s="5" t="s">
@@ -2183,17 +2453,21 @@
       </c>
       <c r="H72" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I72" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Mark Lee</v>
       </c>
     </row>
     <row r="73" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="3">
         <v>41574</v>
       </c>
-      <c r="C73" s="41">
+      <c r="C73" s="40">
         <v>3.3125</v>
       </c>
-      <c r="D73" s="42">
-        <f t="shared" si="1"/>
+      <c r="D73" s="41">
+        <f t="shared" si="2"/>
         <v>41577.3125</v>
       </c>
       <c r="E73" s="5" t="s">
@@ -2201,17 +2475,21 @@
       </c>
       <c r="H73" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I73" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Jouko Haapsaari</v>
       </c>
     </row>
     <row r="74" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="9">
         <v>41577</v>
       </c>
-      <c r="C74" s="41">
+      <c r="C74" s="40">
         <v>3.3541666666666701</v>
       </c>
-      <c r="D74" s="42">
-        <f t="shared" si="1"/>
+      <c r="D74" s="41">
+        <f t="shared" si="2"/>
         <v>41580.354166666664</v>
       </c>
       <c r="E74" s="11"/>
@@ -2222,16 +2500,20 @@
       <c r="H74" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="I74" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
     </row>
     <row r="75" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="3">
         <v>41581</v>
       </c>
-      <c r="C75" s="41">
+      <c r="C75" s="40">
         <v>3.3958333333333299</v>
       </c>
-      <c r="D75" s="42">
-        <f t="shared" si="1"/>
+      <c r="D75" s="41">
+        <f t="shared" si="2"/>
         <v>41584.395833333336</v>
       </c>
       <c r="E75" s="5" t="s">
@@ -2239,17 +2521,21 @@
       </c>
       <c r="H75" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I75" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Ray Waaraniemi</v>
       </c>
     </row>
     <row r="76" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="3">
         <v>41581</v>
       </c>
-      <c r="C76" s="41">
+      <c r="C76" s="40">
         <v>3.4375</v>
       </c>
-      <c r="D76" s="42">
-        <f t="shared" si="1"/>
+      <c r="D76" s="41">
+        <f t="shared" si="2"/>
         <v>41584.4375</v>
       </c>
       <c r="E76" s="5" t="s">
@@ -2257,17 +2543,21 @@
       </c>
       <c r="H76" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I76" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Randy Herrala</v>
       </c>
     </row>
     <row r="77" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="3">
         <v>41584</v>
       </c>
-      <c r="C77" s="41">
+      <c r="C77" s="40">
         <v>3.4791666666666701</v>
       </c>
-      <c r="D77" s="42">
-        <f t="shared" si="1"/>
+      <c r="D77" s="41">
+        <f t="shared" si="2"/>
         <v>41587.479166666664</v>
       </c>
       <c r="E77" s="5" t="s">
@@ -2278,17 +2568,21 @@
       </c>
       <c r="H77" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I77" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Song Services - Rick Nevala</v>
       </c>
     </row>
     <row r="78" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="3">
         <v>41588</v>
       </c>
-      <c r="C78" s="41">
+      <c r="C78" s="40">
         <v>3.5208333333333299</v>
       </c>
-      <c r="D78" s="42">
-        <f t="shared" si="1"/>
+      <c r="D78" s="41">
+        <f t="shared" si="2"/>
         <v>41591.520833333336</v>
       </c>
       <c r="E78" s="5" t="s">
@@ -2296,17 +2590,21 @@
       </c>
       <c r="H78" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I78" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Jouko Haapsaari</v>
       </c>
     </row>
     <row r="79" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="3">
         <v>41588</v>
       </c>
-      <c r="C79" s="41">
+      <c r="C79" s="40">
         <v>3.5625</v>
       </c>
-      <c r="D79" s="42">
-        <f t="shared" si="1"/>
+      <c r="D79" s="41">
+        <f t="shared" si="2"/>
         <v>41591.5625</v>
       </c>
       <c r="E79" s="5" t="s">
@@ -2314,17 +2612,21 @@
       </c>
       <c r="H79" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I79" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Craig Kumpula</v>
       </c>
     </row>
     <row r="80" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="9">
         <v>41591</v>
       </c>
-      <c r="C80" s="41">
+      <c r="C80" s="40">
         <v>3.6041666666666701</v>
       </c>
-      <c r="D80" s="42">
-        <f t="shared" si="1"/>
+      <c r="D80" s="41">
+        <f t="shared" si="2"/>
         <v>41594.604166666664</v>
       </c>
       <c r="E80" s="11"/>
@@ -2335,16 +2637,20 @@
       <c r="H80" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="I80" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
     </row>
     <row r="81" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="3">
         <v>41595</v>
       </c>
-      <c r="C81" s="41">
+      <c r="C81" s="40">
         <v>3.6458333333333299</v>
       </c>
-      <c r="D81" s="42">
-        <f t="shared" si="1"/>
+      <c r="D81" s="41">
+        <f t="shared" si="2"/>
         <v>41598.645833333336</v>
       </c>
       <c r="E81" s="5" t="s">
@@ -2355,17 +2661,21 @@
       </c>
       <c r="H81" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I81" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Service (Rotation Sunday) - John Lehtola</v>
       </c>
     </row>
     <row r="82" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="17">
         <v>41595</v>
       </c>
-      <c r="C82" s="41">
+      <c r="C82" s="40">
         <v>3.6875</v>
       </c>
-      <c r="D82" s="42">
-        <f t="shared" si="1"/>
+      <c r="D82" s="41">
+        <f t="shared" si="2"/>
         <v>41598.6875</v>
       </c>
       <c r="E82" s="19" t="s">
@@ -2376,17 +2686,21 @@
       </c>
       <c r="G82" s="19" t="s">
         <v>52</v>
+      </c>
+      <c r="I82" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>LLCM - Rick Nevala</v>
       </c>
     </row>
     <row r="83" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="3">
         <v>41595</v>
       </c>
-      <c r="C83" s="41">
+      <c r="C83" s="40">
         <v>3.7291666666666701</v>
       </c>
-      <c r="D83" s="42">
-        <f t="shared" si="1"/>
+      <c r="D83" s="41">
+        <f t="shared" si="2"/>
         <v>41598.729166666664</v>
       </c>
       <c r="E83" s="5" t="s">
@@ -2394,17 +2708,21 @@
       </c>
       <c r="H83" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I83" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Jouko Haapsaari</v>
       </c>
     </row>
     <row r="84" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="9">
         <v>41598</v>
       </c>
-      <c r="C84" s="41">
+      <c r="C84" s="40">
         <v>3.7708333333333299</v>
       </c>
-      <c r="D84" s="42">
-        <f t="shared" si="1"/>
+      <c r="D84" s="41">
+        <f t="shared" si="2"/>
         <v>41601.770833333336</v>
       </c>
       <c r="E84" s="11"/>
@@ -2415,16 +2733,20 @@
       <c r="H84" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="I84" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
     </row>
     <row r="85" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="3">
         <v>41602</v>
       </c>
-      <c r="C85" s="41">
+      <c r="C85" s="40">
         <v>3.8125</v>
       </c>
-      <c r="D85" s="42">
-        <f t="shared" si="1"/>
+      <c r="D85" s="41">
+        <f t="shared" si="2"/>
         <v>41605.8125</v>
       </c>
       <c r="E85" s="5" t="s">
@@ -2432,17 +2754,21 @@
       </c>
       <c r="H85" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I85" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Rod Nikula</v>
       </c>
     </row>
     <row r="86" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="17">
         <v>41602</v>
       </c>
-      <c r="C86" s="41">
+      <c r="C86" s="40">
         <v>3.8541666666666701</v>
       </c>
-      <c r="D86" s="42">
-        <f t="shared" si="1"/>
+      <c r="D86" s="41">
+        <f t="shared" si="2"/>
         <v>41605.854166666664</v>
       </c>
       <c r="E86" s="19" t="s">
@@ -2453,17 +2779,21 @@
       </c>
       <c r="G86" s="19" t="s">
         <v>52</v>
+      </c>
+      <c r="I86" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>LLCM - Randy Herrala</v>
       </c>
     </row>
     <row r="87" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="3">
         <v>41602</v>
       </c>
-      <c r="C87" s="41">
+      <c r="C87" s="40">
         <v>3.8958333333333299</v>
       </c>
-      <c r="D87" s="42">
-        <f t="shared" si="1"/>
+      <c r="D87" s="41">
+        <f t="shared" si="2"/>
         <v>41605.895833333336</v>
       </c>
       <c r="E87" s="5" t="s">
@@ -2471,17 +2801,21 @@
       </c>
       <c r="H87" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I87" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Nathan Muhonen</v>
       </c>
     </row>
     <row r="88" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="9">
         <v>41605</v>
       </c>
-      <c r="C88" s="41">
+      <c r="C88" s="40">
         <v>3.9375</v>
       </c>
-      <c r="D88" s="42">
-        <f t="shared" si="1"/>
+      <c r="D88" s="41">
+        <f t="shared" si="2"/>
         <v>41608.9375</v>
       </c>
       <c r="E88" s="11"/>
@@ -2492,16 +2826,20 @@
       <c r="H88" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="I88" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
     </row>
     <row r="89" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="39">
         <v>41606</v>
       </c>
-      <c r="C89" s="41">
+      <c r="C89" s="40">
         <v>3.9791666666666701</v>
       </c>
-      <c r="D89" s="42">
-        <f t="shared" si="1"/>
+      <c r="D89" s="41">
+        <f t="shared" si="2"/>
         <v>41609.979166666664</v>
       </c>
       <c r="E89" s="30" t="s">
@@ -2516,19 +2854,20 @@
       <c r="H89" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="I89" s="30" t="s">
-        <v>76</v>
+      <c r="I89" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Thanksgiving Service - Craig Kumpula</v>
       </c>
     </row>
     <row r="90" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="3">
         <v>41609</v>
       </c>
-      <c r="C90" s="41">
+      <c r="C90" s="40">
         <v>4.0208333333333304</v>
       </c>
-      <c r="D90" s="42">
-        <f t="shared" si="1"/>
+      <c r="D90" s="41">
+        <f t="shared" si="2"/>
         <v>41613.020833333336</v>
       </c>
       <c r="E90" s="5" t="s">
@@ -2536,17 +2875,21 @@
       </c>
       <c r="H90" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I90" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Jouko Haapsaari</v>
       </c>
     </row>
     <row r="91" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="3">
         <v>41609</v>
       </c>
-      <c r="C91" s="41">
+      <c r="C91" s="40">
         <v>4.0625</v>
       </c>
-      <c r="D91" s="42">
-        <f t="shared" si="1"/>
+      <c r="D91" s="41">
+        <f t="shared" si="2"/>
         <v>41613.0625</v>
       </c>
       <c r="E91" s="5" t="s">
@@ -2557,17 +2900,21 @@
       </c>
       <c r="H91" s="5" t="s">
         <v>69</v>
+      </c>
+      <c r="I91" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Advent Program - Mark Lee</v>
       </c>
     </row>
     <row r="92" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="22">
         <v>41609</v>
       </c>
-      <c r="C92" s="41">
+      <c r="C92" s="40">
         <v>4.1041666666666696</v>
       </c>
-      <c r="D92" s="42">
-        <f t="shared" si="1"/>
+      <c r="D92" s="41">
+        <f t="shared" si="2"/>
         <v>41613.104166666664</v>
       </c>
       <c r="E92" s="24" t="s">
@@ -2581,17 +2928,21 @@
       </c>
       <c r="H92" s="24" t="s">
         <v>69</v>
+      </c>
+      <c r="I92" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Annandale Nursing Home  - Joe Lehtola</v>
       </c>
     </row>
     <row r="93" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="22">
         <v>41609</v>
       </c>
-      <c r="C93" s="41">
+      <c r="C93" s="40">
         <v>4.1458333333333304</v>
       </c>
-      <c r="D93" s="42">
-        <f t="shared" si="1"/>
+      <c r="D93" s="41">
+        <f t="shared" si="2"/>
         <v>41613.145833333336</v>
       </c>
       <c r="E93" s="24" t="s">
@@ -2605,17 +2956,21 @@
       </c>
       <c r="H93" s="24" t="s">
         <v>69</v>
+      </c>
+      <c r="I93" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Annandale Nursing Home  - Rick Nevala</v>
       </c>
     </row>
     <row r="94" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="9">
         <v>41612</v>
       </c>
-      <c r="C94" s="41">
+      <c r="C94" s="40">
         <v>4.1875</v>
       </c>
-      <c r="D94" s="42">
-        <f t="shared" si="1"/>
+      <c r="D94" s="41">
+        <f t="shared" si="2"/>
         <v>41616.1875</v>
       </c>
       <c r="E94" s="11"/>
@@ -2626,16 +2981,20 @@
       <c r="H94" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="I94" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Home Services - </v>
+      </c>
     </row>
     <row r="95" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="9">
         <v>41615</v>
       </c>
-      <c r="C95" s="41">
+      <c r="C95" s="40">
         <v>4.2291666666666696</v>
       </c>
-      <c r="D95" s="42">
-        <f t="shared" si="1"/>
+      <c r="D95" s="41">
+        <f t="shared" si="2"/>
         <v>41619.229166666664</v>
       </c>
       <c r="E95" s="11"/>
@@ -2646,16 +3005,20 @@
       <c r="H95" s="5" t="s">
         <v>69</v>
       </c>
+      <c r="I95" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">MBMAC Meeting at RLLC - </v>
+      </c>
     </row>
     <row r="96" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="3">
         <v>41615</v>
       </c>
-      <c r="C96" s="41">
+      <c r="C96" s="40">
         <v>4.2708333333333304</v>
       </c>
-      <c r="D96" s="42">
-        <f t="shared" si="1"/>
+      <c r="D96" s="41">
+        <f t="shared" si="2"/>
         <v>41619.270833333336</v>
       </c>
       <c r="E96" s="5" t="s">
@@ -2667,16 +3030,20 @@
       <c r="H96" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="97" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I96" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Rod Nikula</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="3">
         <v>41616</v>
       </c>
-      <c r="C97" s="41">
+      <c r="C97" s="40">
         <v>4.3125</v>
       </c>
-      <c r="D97" s="42">
-        <f t="shared" si="1"/>
+      <c r="D97" s="41">
+        <f t="shared" si="2"/>
         <v>41620.3125</v>
       </c>
       <c r="E97" s="5" t="s">
@@ -2685,16 +3052,20 @@
       <c r="H97" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="98" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I97" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Ray Waaraniemi</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="3">
         <v>41616</v>
       </c>
-      <c r="C98" s="41">
+      <c r="C98" s="40">
         <v>4.3541666666666696</v>
       </c>
-      <c r="D98" s="42">
-        <f t="shared" si="1"/>
+      <c r="D98" s="41">
+        <f t="shared" si="2"/>
         <v>41620.354166666664</v>
       </c>
       <c r="E98" s="5" t="s">
@@ -2703,16 +3074,20 @@
       <c r="H98" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="99" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I98" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Joe Lehtola</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="3">
         <v>41619</v>
       </c>
-      <c r="C99" s="41">
+      <c r="C99" s="40">
         <v>4.3958333333333304</v>
       </c>
-      <c r="D99" s="42">
-        <f t="shared" si="1"/>
+      <c r="D99" s="41">
+        <f t="shared" si="2"/>
         <v>41623.395833333336</v>
       </c>
       <c r="E99" s="5" t="s">
@@ -2724,16 +3099,20 @@
       <c r="H99" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="100" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I99" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Christmas Song Services - Rick Nevala</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="3">
         <v>41623</v>
       </c>
-      <c r="C100" s="41">
+      <c r="C100" s="40">
         <v>4.4375</v>
       </c>
-      <c r="D100" s="42">
-        <f t="shared" si="1"/>
+      <c r="D100" s="41">
+        <f t="shared" si="2"/>
         <v>41627.4375</v>
       </c>
       <c r="E100" s="5" t="s">
@@ -2742,16 +3121,20 @@
       <c r="H100" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="101" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I100" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Rocky Sorvala</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="17">
         <v>41623</v>
       </c>
-      <c r="C101" s="41">
+      <c r="C101" s="40">
         <v>4.4791666666666696</v>
       </c>
-      <c r="D101" s="42">
-        <f t="shared" si="1"/>
+      <c r="D101" s="41">
+        <f t="shared" si="2"/>
         <v>41627.479166666664</v>
       </c>
       <c r="E101" s="19" t="s">
@@ -2763,16 +3146,20 @@
       <c r="G101" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="102" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I101" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>LLCM - Craig Kumpula</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="3">
         <v>41623</v>
       </c>
-      <c r="C102" s="41">
+      <c r="C102" s="40">
         <v>4.5208333333333304</v>
       </c>
-      <c r="D102" s="42">
-        <f t="shared" si="1"/>
+      <c r="D102" s="41">
+        <f t="shared" si="2"/>
         <v>41627.520833333336</v>
       </c>
       <c r="E102" s="5" t="s">
@@ -2787,16 +3174,20 @@
       <c r="H102" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="103" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I102" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Sunday School Christmas Program - Randy Herrala</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="9">
         <v>41626</v>
       </c>
-      <c r="C103" s="41">
+      <c r="C103" s="40">
         <v>4.5625</v>
       </c>
-      <c r="D103" s="42">
-        <f t="shared" si="1"/>
+      <c r="D103" s="41">
+        <f t="shared" si="2"/>
         <v>41630.5625</v>
       </c>
       <c r="E103" s="11"/>
@@ -2807,16 +3198,20 @@
       <c r="H103" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="104" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I103" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">Bible Class - </v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="3">
         <v>41630</v>
       </c>
-      <c r="C104" s="41">
+      <c r="C104" s="40">
         <v>4.6041666666666696</v>
       </c>
-      <c r="D104" s="42">
-        <f t="shared" si="1"/>
+      <c r="D104" s="41">
+        <f t="shared" si="2"/>
         <v>41634.604166666664</v>
       </c>
       <c r="E104" s="5" t="s">
@@ -2825,16 +3220,20 @@
       <c r="H104" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="105" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I104" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Mark Lee</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="3">
         <v>41630</v>
       </c>
-      <c r="C105" s="41">
+      <c r="C105" s="40">
         <v>4.6458333333333304</v>
       </c>
-      <c r="D105" s="42">
-        <f t="shared" si="1"/>
+      <c r="D105" s="41">
+        <f t="shared" si="2"/>
         <v>41634.645833333336</v>
       </c>
       <c r="E105" s="5" t="s">
@@ -2843,16 +3242,20 @@
       <c r="H105" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="106" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I105" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Nathan Muhonen</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B106" s="17">
         <v>41630</v>
       </c>
-      <c r="C106" s="41">
+      <c r="C106" s="40">
         <v>4.6875</v>
       </c>
-      <c r="D106" s="42">
-        <f t="shared" si="1"/>
+      <c r="D106" s="41">
+        <f t="shared" si="2"/>
         <v>41634.6875</v>
       </c>
       <c r="E106" s="19" t="s">
@@ -2864,16 +3267,20 @@
       <c r="G106" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="107" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I106" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>LLCM - Randy Herrala</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B107" s="3">
         <v>41632</v>
       </c>
-      <c r="C107" s="41">
+      <c r="C107" s="40">
         <v>4.7291666666666696</v>
       </c>
-      <c r="D107" s="42">
-        <f t="shared" si="1"/>
+      <c r="D107" s="41">
+        <f t="shared" si="2"/>
         <v>41636.729166666664</v>
       </c>
       <c r="E107" s="5" t="s">
@@ -2885,16 +3292,20 @@
       <c r="H107" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="108" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I107" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Christmas Eve Service - Rod Nikula</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B108" s="3">
         <v>41632</v>
       </c>
-      <c r="C108" s="41">
+      <c r="C108" s="40">
         <v>4.7708333333333304</v>
       </c>
-      <c r="D108" s="42">
-        <f t="shared" si="1"/>
+      <c r="D108" s="41">
+        <f t="shared" si="2"/>
         <v>41636.770833333336</v>
       </c>
       <c r="E108" s="5" t="s">
@@ -2906,16 +3317,20 @@
       <c r="H108" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="109" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I108" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Christmas Eve Service - Craig Kumpula</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B109" s="3">
         <v>41633</v>
       </c>
-      <c r="C109" s="41">
+      <c r="C109" s="40">
         <v>4.8125</v>
       </c>
-      <c r="D109" s="42">
-        <f t="shared" si="1"/>
+      <c r="D109" s="41">
+        <f t="shared" si="2"/>
         <v>41637.8125</v>
       </c>
       <c r="E109" s="5" t="s">
@@ -2927,16 +3342,20 @@
       <c r="H109" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="110" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I109" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Christmas Day Service - Joe Lehtola</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B110" s="3">
         <v>41633</v>
       </c>
-      <c r="C110" s="41">
+      <c r="C110" s="40">
         <v>4.8541666666666696</v>
       </c>
-      <c r="D110" s="42">
-        <f t="shared" si="1"/>
+      <c r="D110" s="41">
+        <f t="shared" si="2"/>
         <v>41637.854166666664</v>
       </c>
       <c r="E110" s="5" t="s">
@@ -2948,16 +3367,20 @@
       <c r="H110" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="111" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I110" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Christmas Day Service - Rocky Sorvala</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B111" s="3">
         <v>41637</v>
       </c>
-      <c r="C111" s="41">
+      <c r="C111" s="40">
         <v>4.8958333333333304</v>
       </c>
-      <c r="D111" s="42">
-        <f t="shared" si="1"/>
+      <c r="D111" s="41">
+        <f t="shared" si="2"/>
         <v>41641.895833333336</v>
       </c>
       <c r="E111" s="5" t="s">
@@ -2966,16 +3389,20 @@
       <c r="H111" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="112" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I111" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Rick Nevala</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B112" s="17">
         <v>41637</v>
       </c>
-      <c r="C112" s="41">
+      <c r="C112" s="40">
         <v>4.9375</v>
       </c>
-      <c r="D112" s="42">
-        <f t="shared" si="1"/>
+      <c r="D112" s="41">
+        <f t="shared" si="2"/>
         <v>41641.9375</v>
       </c>
       <c r="E112" s="19" t="s">
@@ -2987,16 +3414,20 @@
       <c r="G112" s="19" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="113" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I112" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>LLCM - Joe Lehtola</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B113" s="3">
         <v>41637</v>
       </c>
-      <c r="C113" s="41">
+      <c r="C113" s="40">
         <v>4.9791666666666696</v>
       </c>
-      <c r="D113" s="42">
-        <f t="shared" si="1"/>
+      <c r="D113" s="41">
+        <f t="shared" si="2"/>
         <v>41641.979166666664</v>
       </c>
       <c r="E113" s="5" t="s">
@@ -3005,16 +3436,20 @@
       <c r="H113" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="114" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I113" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Ray Waaraniemi</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B114" s="3">
         <v>41639</v>
       </c>
-      <c r="C114" s="41">
+      <c r="C114" s="40">
         <v>5.0208333333333304</v>
       </c>
-      <c r="D114" s="42">
-        <f t="shared" si="1"/>
+      <c r="D114" s="41">
+        <f t="shared" si="2"/>
         <v>41644.020833333336</v>
       </c>
       <c r="E114" s="5" t="s">
@@ -3026,16 +3461,20 @@
       <c r="H114" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="115" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I114" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>New Years Eve Services - Mark Lee</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B115" s="3">
         <v>41639</v>
       </c>
-      <c r="C115" s="41">
+      <c r="C115" s="40">
         <v>5.0625</v>
       </c>
-      <c r="D115" s="42">
-        <f t="shared" si="1"/>
+      <c r="D115" s="41">
+        <f t="shared" si="2"/>
         <v>41644.0625</v>
       </c>
       <c r="E115" s="5" t="s">
@@ -3050,16 +3489,20 @@
       <c r="H115" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="116" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I115" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>New Years Eve Services - Nathan Muhonen</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B116" s="3">
         <v>41640</v>
       </c>
-      <c r="C116" s="41">
+      <c r="C116" s="40">
         <v>5.1041666666666696</v>
       </c>
-      <c r="D116" s="42">
-        <f t="shared" si="1"/>
+      <c r="D116" s="41">
+        <f t="shared" si="2"/>
         <v>41645.104166666664</v>
       </c>
       <c r="E116" s="5" t="s">
@@ -3071,16 +3514,20 @@
       <c r="H116" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="117" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I116" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>New Years Day - Jouko Haapsaari</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B117" s="3">
         <v>41644</v>
       </c>
-      <c r="C117" s="41">
+      <c r="C117" s="40">
         <v>5.1458333333333304</v>
       </c>
-      <c r="D117" s="42">
-        <f t="shared" si="1"/>
+      <c r="D117" s="41">
+        <f t="shared" si="2"/>
         <v>41649.145833333336</v>
       </c>
       <c r="E117" s="5" t="s">
@@ -3089,32 +3536,40 @@
       <c r="H117" s="5" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="118" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I117" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Randy Herrala</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="3">
         <v>41644</v>
       </c>
-      <c r="C118" s="41">
+      <c r="C118" s="40">
         <v>5.1875</v>
       </c>
-      <c r="D118" s="42">
-        <f t="shared" si="1"/>
+      <c r="D118" s="41">
+        <f t="shared" si="2"/>
         <v>41649.1875</v>
       </c>
       <c r="E118" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="119" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" spans="2:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="I118" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve"> - Rod Nikula</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="129" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="130" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>